<commit_message>
finsihed order && notification
</commit_message>
<xml_diff>
--- a/files/product.xlsx
+++ b/files/product.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\php7.2\xampp\htdocs\aghezty_php7\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\php7.2\xampp\htdocs\aghezty_v2_php7\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>description_ar</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>1_1.png,1_2.png,1_3.png</t>
+  </si>
+  <si>
+    <t>inch</t>
   </si>
 </sst>
 </file>
@@ -121,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +139,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -168,7 +177,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -177,6 +186,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -459,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:XFD3"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +490,7 @@
     <col min="14" max="14" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -517,8 +527,11 @@
       <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -554,6 +567,9 @@
       </c>
       <c r="L2" t="s">
         <v>19</v>
+      </c>
+      <c r="M2">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add sku && fix some issue
</commit_message>
<xml_diff>
--- a/files/product.xlsx
+++ b/files/product.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>description_ar</t>
   </si>
@@ -50,12 +50,6 @@
     <t>stock</t>
   </si>
   <si>
-    <t>special</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
     <t>main_image</t>
   </si>
   <si>
@@ -74,19 +68,28 @@
     <t>Model En</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>1.jpg</t>
   </si>
   <si>
     <t>1_1.png,1_2.png,1_3.png</t>
   </si>
   <si>
-    <t>inch</t>
+    <t>title_en</t>
+  </si>
+  <si>
+    <t>title_ar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Put Your Title Arabic Here </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Put Your Title English Here </t>
+  </si>
+  <si>
+    <t>sku</t>
+  </si>
+  <si>
+    <t>optional value</t>
   </si>
 </sst>
 </file>
@@ -124,7 +127,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,14 +144,8 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -171,13 +168,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -186,7 +198,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -471,19 +486,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="36.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="1" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
     <col min="11" max="11" width="25.42578125" customWidth="1"/>
     <col min="12" max="12" width="29.5703125" customWidth="1"/>
     <col min="13" max="13" width="24" customWidth="1"/>
@@ -491,85 +507,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2">
+        <v>1000</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>990</v>
+      </c>
+      <c r="J2">
+        <v>40</v>
+      </c>
+      <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="L2" t="s">
         <v>15</v>
       </c>
-      <c r="E2">
-        <v>1000</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>990</v>
-      </c>
-      <c r="H2">
-        <v>40</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2">
-        <v>32</v>
+      <c r="M2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>